<commit_message>
Update all the notebooks
</commit_message>
<xml_diff>
--- a/2_BoW_Models/1_MLP/BoW_MLP_MPQA_3.xlsx
+++ b/2_BoW_Models/1_MLP/BoW_MLP_MPQA_3.xlsx
@@ -1,37 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diardano Raihan\Documents\My Life\AI\Portofolio\Text_Classification_Capstone\2_BoW_Models\1_MLP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4937DC06-CA50-46DF-A67A-683574CEEF32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="model_3" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="model_3" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>tfidf</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +72,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,212 +397,219 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>binary</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>count</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>tfidf</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>freq</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.8435438275337219</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.8501413464546204</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.8557963967323303</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.8331762552261353</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>0.871819019317627</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.8520264029502869</v>
-      </c>
-      <c r="D3" t="n">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.84354382753372192</v>
+      </c>
+      <c r="C2">
+        <v>0.85014134645462036</v>
+      </c>
+      <c r="D2">
+        <v>0.85579639673233032</v>
+      </c>
+      <c r="E2">
+        <v>0.83317625522613525</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.87181901931762695</v>
+      </c>
+      <c r="C3">
+        <v>0.85202640295028687</v>
+      </c>
+      <c r="D3">
         <v>0.8416588306427002</v>
       </c>
-      <c r="E3" t="n">
-        <v>0.8623939752578735</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="E3">
+        <v>0.86239397525787354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>0.8388313055038452</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.8633365035057068</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="B4">
+        <v>0.83883130550384521</v>
+      </c>
+      <c r="C4">
+        <v>0.86333650350570679</v>
+      </c>
+      <c r="D4">
         <v>0.8586239218711853</v>
       </c>
-      <c r="E4" t="n">
-        <v>0.8623939752578735</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="E4">
+        <v>0.86239397525787354</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
-        <v>0.8633365035057068</v>
-      </c>
-      <c r="C5" t="n">
+      <c r="B5">
+        <v>0.86333650350570679</v>
+      </c>
+      <c r="C5">
         <v>0.8586239218711853</v>
       </c>
-      <c r="D5" t="n">
-        <v>0.8256362080574036</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.8501413464546204</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="D5">
+        <v>0.82563620805740356</v>
+      </c>
+      <c r="E5">
+        <v>0.85014134645462036</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
-        <v>0.8548539280891418</v>
-      </c>
-      <c r="C6" t="n">
+      <c r="B6">
+        <v>0.85485392808914185</v>
+      </c>
+      <c r="C6">
         <v>0.8416588306427002</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>0.8463713526725769</v>
       </c>
-      <c r="E6" t="n">
-        <v>0.8567389249801636</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="E6">
+        <v>0.85673892498016357</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
-        <v>0.8708765506744385</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.8557963967323303</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.8576814532279968</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.8595664501190186</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="B7">
+        <v>0.87087655067443848</v>
+      </c>
+      <c r="C7">
+        <v>0.85579639673233032</v>
+      </c>
+      <c r="D7">
+        <v>0.85768145322799683</v>
+      </c>
+      <c r="E7">
+        <v>0.85956645011901855</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
-        <v>0.849056601524353</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.8320754766464233</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.8443396091461182</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.850943386554718</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="B8">
+        <v>0.84905660152435303</v>
+      </c>
+      <c r="C8">
+        <v>0.83207547664642334</v>
+      </c>
+      <c r="D8">
+        <v>0.84433960914611816</v>
+      </c>
+      <c r="E8">
+        <v>0.85094338655471802</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>0.8518868088722229</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.8764150738716125</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="C9">
+        <v>0.87641507387161255</v>
+      </c>
+      <c r="D9">
         <v>0.8669811487197876</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>0.854716956615448</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
-        <v>0.8584905862808228</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.8566038012504578</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.8679245114326477</v>
-      </c>
-      <c r="E10" t="n">
+      <c r="B10">
+        <v>0.85849058628082275</v>
+      </c>
+      <c r="C10">
+        <v>0.85660380125045776</v>
+      </c>
+      <c r="D10">
+        <v>0.86792451143264771</v>
+      </c>
+      <c r="E10">
         <v>0.8518868088722229</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="n">
-        <v>0.8603773713111877</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.850943386554718</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.8566038012504578</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.8603773713111877</v>
+      <c r="B11">
+        <v>0.86037737131118774</v>
+      </c>
+      <c r="C11">
+        <v>0.85094338655471802</v>
+      </c>
+      <c r="D11">
+        <v>0.85660380125045776</v>
+      </c>
+      <c r="E11">
+        <v>0.86037737131118774</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="2">
+        <f>AVERAGE(B2:B11)*100</f>
+        <v>85.630725026130676</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" ref="C12:E12" si="0">AVERAGE(C2:C11)*100</f>
+        <v>85.376211404800415</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>85.216172337532043</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>85.423354506492615</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>